<commit_message>
Retrieve YOLO model metrics code
</commit_message>
<xml_diff>
--- a/Runs/RunsLog.xlsx
+++ b/Runs/RunsLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cguenther\AIBootcamp\Classwork\Project3_backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B546AC4F-2F59-4BAD-A444-1F83F898DB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA69391C-A30A-41C3-B199-242BBB7A62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C77497C3-59A1-4AFE-A6BB-B1978551ABAD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>AdamW</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Mediaum_model_2</t>
   </si>
   <si>
     <t>Medium_model_3</t>
@@ -254,6 +251,9 @@
     <t>1 class
 Continue previous medium run for total 900 epochs
 Finished early after 100 epochs w/o progress</t>
+  </si>
+  <si>
+    <t>Medium_model_2</t>
   </si>
 </sst>
 </file>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9B80FA-0180-49A3-AD1C-64A783CC99B1}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,31 +691,31 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -745,10 +745,10 @@
         <v>13</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>15</v>
@@ -804,13 +804,13 @@
         <v>14</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -860,16 +860,16 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -919,21 +919,21 @@
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>1487</v>
@@ -978,21 +978,21 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1487</v>
@@ -1037,16 +1037,16 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -1105,16 +1105,16 @@
         <v>1</v>
       </c>
       <c r="S7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -1173,16 +1173,16 @@
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="58" x14ac:dyDescent="0.35">
@@ -1242,16 +1242,16 @@
         <v>1</v>
       </c>
       <c r="S9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="58" x14ac:dyDescent="0.35">
@@ -1311,16 +1311,16 @@
         <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="58" x14ac:dyDescent="0.35">
@@ -1380,21 +1380,21 @@
         <v>1</v>
       </c>
       <c r="S11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>8145</v>
@@ -1449,18 +1449,21 @@
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>8145</v>
@@ -1515,21 +1518,21 @@
         <v>1</v>
       </c>
       <c r="S13" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>8145</v>
@@ -1584,21 +1587,21 @@
         <v>1</v>
       </c>
       <c r="S14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>8145</v>
@@ -1653,21 +1656,21 @@
         <v>1</v>
       </c>
       <c r="S15" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>8145</v>
@@ -1722,21 +1725,21 @@
         <v>1</v>
       </c>
       <c r="S16" t="s">
+        <v>54</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>8145</v>
@@ -1791,21 +1794,21 @@
         <v>1</v>
       </c>
       <c r="S17" t="s">
+        <v>56</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>8145</v>
@@ -1860,16 +1863,16 @@
         <v>1</v>
       </c>
       <c r="S18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V18" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>